<commit_message>
kadın erkek bar plot & pie chart
</commit_message>
<xml_diff>
--- a/veri/Kadin_Erkek_Yas_Dagilimlari_Turkiye.xlsx
+++ b/veri/Kadin_Erkek_Yas_Dagilimlari_Turkiye.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20417"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zahide\Desktop\yeni veri seti - bölge\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BUSENUR\Documents\GitHub\muy665-bahar2025-takim-R_amam_soRmam_biR_daha\veri\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{80DB6241-C077-4681-86FE-31391DAE5AD8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B3C58A1-1F4B-4FAC-8597-78779B067532}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{A6048D78-C244-48EB-83DB-3DD76459F337}"/>
+    <workbookView xWindow="3495" yWindow="2775" windowWidth="15375" windowHeight="7875" activeTab="1" xr2:uid="{A6048D78-C244-48EB-83DB-3DD76459F337}"/>
   </bookViews>
   <sheets>
     <sheet name="Kadın Yaş Dağılımı" sheetId="2" r:id="rId1"/>
@@ -95,19 +95,7 @@
     <t>2024</t>
   </si>
   <si>
-    <t>Yas_16_29</t>
-  </si>
-  <si>
-    <t>Yas_30_44</t>
-  </si>
-  <si>
-    <t>Yas_55_60ustu</t>
-  </si>
-  <si>
     <t>Yil</t>
-  </si>
-  <si>
-    <t>Yas_45_54</t>
   </si>
   <si>
     <t>TÜRKİYE</t>
@@ -117,6 +105,18 @@
   </si>
   <si>
     <t>Yas_Grubu</t>
+  </si>
+  <si>
+    <t>Yaş Aralığı: 16-29</t>
+  </si>
+  <si>
+    <t>Yaş Aralığı: 30-44</t>
+  </si>
+  <si>
+    <t>Yaş Aralığı: 45-54</t>
+  </si>
+  <si>
+    <t>Yaş Aralığı: 55 ve 60 üstü</t>
   </si>
 </sst>
 </file>
@@ -511,12 +511,12 @@
   <dimension ref="A1:C98"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="26.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.28515625" style="1" customWidth="1"/>
     <col min="3" max="3" width="11.5703125" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
@@ -531,19 +531,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
-        <v>31</v>
+      <c r="A1" s="1" t="s">
+        <v>27</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -554,7 +554,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
@@ -565,7 +565,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B4" t="s">
         <v>2</v>
@@ -576,7 +576,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B5" t="s">
         <v>3</v>
@@ -587,7 +587,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B6" t="s">
         <v>4</v>
@@ -598,7 +598,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B7" t="s">
         <v>5</v>
@@ -609,7 +609,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B8" t="s">
         <v>6</v>
@@ -620,7 +620,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B9" t="s">
         <v>7</v>
@@ -631,7 +631,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B10" t="s">
         <v>8</v>
@@ -642,7 +642,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B11" t="s">
         <v>9</v>
@@ -653,7 +653,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B12" t="s">
         <v>10</v>
@@ -664,7 +664,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B13" t="s">
         <v>11</v>
@@ -675,7 +675,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B14" t="s">
         <v>12</v>
@@ -686,7 +686,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B15" t="s">
         <v>13</v>
@@ -697,7 +697,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B16" t="s">
         <v>14</v>
@@ -708,7 +708,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B17" t="s">
         <v>15</v>
@@ -719,7 +719,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B18" t="s">
         <v>16</v>
@@ -730,7 +730,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B19" t="s">
         <v>17</v>
@@ -741,7 +741,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B20" t="s">
         <v>18</v>
@@ -752,7 +752,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B21" t="s">
         <v>19</v>
@@ -763,7 +763,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B22" t="s">
         <v>20</v>
@@ -774,7 +774,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B23" t="s">
         <v>21</v>
@@ -785,7 +785,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B24" t="s">
         <v>22</v>
@@ -796,7 +796,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B25" t="s">
         <v>23</v>
@@ -807,7 +807,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B26" t="s">
         <v>0</v>
@@ -818,7 +818,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B27" t="s">
         <v>1</v>
@@ -829,7 +829,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B28" t="s">
         <v>2</v>
@@ -840,7 +840,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B29" t="s">
         <v>3</v>
@@ -851,7 +851,7 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B30" t="s">
         <v>4</v>
@@ -862,7 +862,7 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B31" t="s">
         <v>5</v>
@@ -873,7 +873,7 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B32" t="s">
         <v>6</v>
@@ -884,7 +884,7 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B33" t="s">
         <v>7</v>
@@ -895,7 +895,7 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B34" t="s">
         <v>8</v>
@@ -906,7 +906,7 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B35" t="s">
         <v>9</v>
@@ -917,7 +917,7 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B36" t="s">
         <v>10</v>
@@ -928,7 +928,7 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B37" t="s">
         <v>11</v>
@@ -939,7 +939,7 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B38" t="s">
         <v>12</v>
@@ -950,7 +950,7 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B39" t="s">
         <v>13</v>
@@ -961,7 +961,7 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B40" t="s">
         <v>14</v>
@@ -972,7 +972,7 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B41" t="s">
         <v>15</v>
@@ -983,7 +983,7 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B42" t="s">
         <v>16</v>
@@ -994,7 +994,7 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B43" t="s">
         <v>17</v>
@@ -1005,7 +1005,7 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B44" t="s">
         <v>18</v>
@@ -1016,7 +1016,7 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B45" t="s">
         <v>19</v>
@@ -1027,7 +1027,7 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B46" t="s">
         <v>20</v>
@@ -1038,7 +1038,7 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B47" t="s">
         <v>21</v>
@@ -1049,7 +1049,7 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B48" t="s">
         <v>22</v>
@@ -1060,7 +1060,7 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B49" t="s">
         <v>23</v>
@@ -1071,7 +1071,7 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B50" t="s">
         <v>0</v>
@@ -1082,7 +1082,7 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B51" t="s">
         <v>1</v>
@@ -1093,7 +1093,7 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B52" t="s">
         <v>2</v>
@@ -1104,7 +1104,7 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B53" t="s">
         <v>3</v>
@@ -1115,7 +1115,7 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B54" t="s">
         <v>4</v>
@@ -1126,7 +1126,7 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B55" t="s">
         <v>5</v>
@@ -1137,7 +1137,7 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B56" t="s">
         <v>6</v>
@@ -1148,7 +1148,7 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B57" t="s">
         <v>7</v>
@@ -1159,7 +1159,7 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B58" t="s">
         <v>8</v>
@@ -1170,7 +1170,7 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B59" t="s">
         <v>9</v>
@@ -1181,7 +1181,7 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B60" t="s">
         <v>10</v>
@@ -1192,7 +1192,7 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B61" t="s">
         <v>11</v>
@@ -1203,7 +1203,7 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B62" t="s">
         <v>12</v>
@@ -1214,7 +1214,7 @@
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B63" t="s">
         <v>13</v>
@@ -1225,7 +1225,7 @@
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B64" t="s">
         <v>14</v>
@@ -1236,7 +1236,7 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B65" t="s">
         <v>15</v>
@@ -1247,7 +1247,7 @@
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B66" t="s">
         <v>16</v>
@@ -1258,7 +1258,7 @@
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B67" t="s">
         <v>17</v>
@@ -1269,7 +1269,7 @@
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B68" t="s">
         <v>18</v>
@@ -1280,7 +1280,7 @@
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B69" t="s">
         <v>19</v>
@@ -1291,7 +1291,7 @@
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B70" t="s">
         <v>20</v>
@@ -1302,7 +1302,7 @@
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B71" t="s">
         <v>21</v>
@@ -1313,7 +1313,7 @@
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B72" t="s">
         <v>22</v>
@@ -1324,7 +1324,7 @@
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B73" t="s">
         <v>23</v>
@@ -1335,7 +1335,7 @@
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74" s="2" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B74" t="s">
         <v>0</v>
@@ -1346,7 +1346,7 @@
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" s="2" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B75" t="s">
         <v>1</v>
@@ -1357,7 +1357,7 @@
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76" s="2" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B76" t="s">
         <v>2</v>
@@ -1368,7 +1368,7 @@
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77" s="2" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B77" t="s">
         <v>3</v>
@@ -1379,7 +1379,7 @@
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78" s="2" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B78" t="s">
         <v>4</v>
@@ -1390,7 +1390,7 @@
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79" s="2" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B79" t="s">
         <v>5</v>
@@ -1401,7 +1401,7 @@
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80" s="2" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B80" t="s">
         <v>6</v>
@@ -1412,7 +1412,7 @@
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81" s="2" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B81" t="s">
         <v>7</v>
@@ -1423,7 +1423,7 @@
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82" s="2" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B82" t="s">
         <v>8</v>
@@ -1434,7 +1434,7 @@
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A83" s="2" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B83" t="s">
         <v>9</v>
@@ -1445,7 +1445,7 @@
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A84" s="2" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B84" t="s">
         <v>10</v>
@@ -1456,7 +1456,7 @@
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A85" s="2" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B85" t="s">
         <v>11</v>
@@ -1467,7 +1467,7 @@
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A86" s="2" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B86" t="s">
         <v>12</v>
@@ -1478,7 +1478,7 @@
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A87" s="2" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B87" t="s">
         <v>13</v>
@@ -1489,7 +1489,7 @@
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A88" s="2" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B88" t="s">
         <v>14</v>
@@ -1500,7 +1500,7 @@
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A89" s="2" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B89" t="s">
         <v>15</v>
@@ -1511,7 +1511,7 @@
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A90" s="2" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B90" t="s">
         <v>16</v>
@@ -1522,7 +1522,7 @@
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A91" s="2" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B91" t="s">
         <v>17</v>
@@ -1533,7 +1533,7 @@
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A92" s="2" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B92" t="s">
         <v>18</v>
@@ -1544,7 +1544,7 @@
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A93" s="2" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B93" t="s">
         <v>19</v>
@@ -1555,7 +1555,7 @@
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A94" s="2" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B94" t="s">
         <v>20</v>
@@ -1566,7 +1566,7 @@
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A95" s="2" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B95" t="s">
         <v>21</v>
@@ -1577,7 +1577,7 @@
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A96" s="2" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B96" t="s">
         <v>22</v>
@@ -1588,7 +1588,7 @@
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A97" s="2" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B97" t="s">
         <v>23</v>
@@ -1608,9 +1608,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E99E99D6-B1E8-4DFD-96F0-1796B7E6A3F8}">
   <dimension ref="A1:C98"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2641,18 +2639,18 @@
   <sheetData>
     <row r="1" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B2" s="1">
         <v>2001</v>
@@ -2663,7 +2661,7 @@
     </row>
     <row r="3" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>1</v>
@@ -2674,7 +2672,7 @@
     </row>
     <row r="4" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>2</v>
@@ -2685,7 +2683,7 @@
     </row>
     <row r="5" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>3</v>
@@ -2696,7 +2694,7 @@
     </row>
     <row r="6" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>4</v>
@@ -2707,7 +2705,7 @@
     </row>
     <row r="7" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>5</v>
@@ -2718,7 +2716,7 @@
     </row>
     <row r="8" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>6</v>
@@ -2729,7 +2727,7 @@
     </row>
     <row r="9" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>7</v>
@@ -2740,7 +2738,7 @@
     </row>
     <row r="10" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>8</v>
@@ -2751,7 +2749,7 @@
     </row>
     <row r="11" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>9</v>
@@ -2762,7 +2760,7 @@
     </row>
     <row r="12" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>10</v>
@@ -2773,7 +2771,7 @@
     </row>
     <row r="13" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>11</v>
@@ -2784,7 +2782,7 @@
     </row>
     <row r="14" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>12</v>
@@ -2795,7 +2793,7 @@
     </row>
     <row r="15" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>13</v>
@@ -2806,7 +2804,7 @@
     </row>
     <row r="16" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>14</v>
@@ -2817,7 +2815,7 @@
     </row>
     <row r="17" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>15</v>
@@ -2828,7 +2826,7 @@
     </row>
     <row r="18" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>16</v>
@@ -2839,7 +2837,7 @@
     </row>
     <row r="19" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>17</v>
@@ -2850,7 +2848,7 @@
     </row>
     <row r="20" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>18</v>
@@ -2861,7 +2859,7 @@
     </row>
     <row r="21" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>19</v>
@@ -2872,7 +2870,7 @@
     </row>
     <row r="22" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>20</v>
@@ -2883,7 +2881,7 @@
     </row>
     <row r="23" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>21</v>
@@ -2894,7 +2892,7 @@
     </row>
     <row r="24" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>22</v>
@@ -2905,7 +2903,7 @@
     </row>
     <row r="25" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>23</v>
@@ -2916,7 +2914,7 @@
     </row>
     <row r="26" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>0</v>
@@ -2927,7 +2925,7 @@
     </row>
     <row r="27" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>1</v>
@@ -2938,7 +2936,7 @@
     </row>
     <row r="28" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>2</v>
@@ -2949,7 +2947,7 @@
     </row>
     <row r="29" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>3</v>
@@ -2960,7 +2958,7 @@
     </row>
     <row r="30" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>4</v>
@@ -2971,7 +2969,7 @@
     </row>
     <row r="31" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>5</v>
@@ -2982,7 +2980,7 @@
     </row>
     <row r="32" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>6</v>
@@ -2993,7 +2991,7 @@
     </row>
     <row r="33" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>7</v>
@@ -3004,7 +3002,7 @@
     </row>
     <row r="34" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>8</v>
@@ -3015,7 +3013,7 @@
     </row>
     <row r="35" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>9</v>
@@ -3026,7 +3024,7 @@
     </row>
     <row r="36" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>10</v>
@@ -3037,7 +3035,7 @@
     </row>
     <row r="37" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>11</v>
@@ -3048,7 +3046,7 @@
     </row>
     <row r="38" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>12</v>
@@ -3059,7 +3057,7 @@
     </row>
     <row r="39" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>13</v>
@@ -3070,7 +3068,7 @@
     </row>
     <row r="40" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>14</v>
@@ -3081,7 +3079,7 @@
     </row>
     <row r="41" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>15</v>
@@ -3092,7 +3090,7 @@
     </row>
     <row r="42" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>16</v>
@@ -3103,7 +3101,7 @@
     </row>
     <row r="43" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>17</v>
@@ -3114,7 +3112,7 @@
     </row>
     <row r="44" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>18</v>
@@ -3125,7 +3123,7 @@
     </row>
     <row r="45" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>19</v>
@@ -3136,7 +3134,7 @@
     </row>
     <row r="46" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>20</v>
@@ -3147,7 +3145,7 @@
     </row>
     <row r="47" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>21</v>
@@ -3158,7 +3156,7 @@
     </row>
     <row r="48" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>22</v>
@@ -3169,7 +3167,7 @@
     </row>
     <row r="49" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>23</v>
@@ -3180,7 +3178,7 @@
     </row>
     <row r="50" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>0</v>
@@ -3191,7 +3189,7 @@
     </row>
     <row r="51" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>1</v>
@@ -3202,7 +3200,7 @@
     </row>
     <row r="52" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>2</v>
@@ -3213,7 +3211,7 @@
     </row>
     <row r="53" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>3</v>
@@ -3224,7 +3222,7 @@
     </row>
     <row r="54" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>4</v>
@@ -3235,7 +3233,7 @@
     </row>
     <row r="55" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>5</v>
@@ -3246,7 +3244,7 @@
     </row>
     <row r="56" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>6</v>
@@ -3257,7 +3255,7 @@
     </row>
     <row r="57" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>7</v>
@@ -3268,7 +3266,7 @@
     </row>
     <row r="58" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>8</v>
@@ -3279,7 +3277,7 @@
     </row>
     <row r="59" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>9</v>
@@ -3290,7 +3288,7 @@
     </row>
     <row r="60" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>10</v>
@@ -3301,7 +3299,7 @@
     </row>
     <row r="61" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>11</v>
@@ -3312,7 +3310,7 @@
     </row>
     <row r="62" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>12</v>
@@ -3323,7 +3321,7 @@
     </row>
     <row r="63" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>13</v>
@@ -3334,7 +3332,7 @@
     </row>
     <row r="64" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>14</v>
@@ -3345,7 +3343,7 @@
     </row>
     <row r="65" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B65" s="1" t="s">
         <v>15</v>
@@ -3356,7 +3354,7 @@
     </row>
     <row r="66" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>16</v>
@@ -3367,7 +3365,7 @@
     </row>
     <row r="67" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>17</v>
@@ -3378,7 +3376,7 @@
     </row>
     <row r="68" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>18</v>
@@ -3389,7 +3387,7 @@
     </row>
     <row r="69" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B69" s="1" t="s">
         <v>19</v>
@@ -3400,7 +3398,7 @@
     </row>
     <row r="70" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B70" s="1" t="s">
         <v>20</v>
@@ -3411,7 +3409,7 @@
     </row>
     <row r="71" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B71" s="1" t="s">
         <v>21</v>
@@ -3422,7 +3420,7 @@
     </row>
     <row r="72" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B72" s="1" t="s">
         <v>22</v>
@@ -3433,7 +3431,7 @@
     </row>
     <row r="73" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B73" s="1" t="s">
         <v>23</v>
@@ -3444,7 +3442,7 @@
     </row>
     <row r="74" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="2" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B74" s="1" t="s">
         <v>0</v>
@@ -3455,7 +3453,7 @@
     </row>
     <row r="75" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="2" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B75" s="1" t="s">
         <v>1</v>
@@ -3466,7 +3464,7 @@
     </row>
     <row r="76" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="2" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B76" s="1" t="s">
         <v>2</v>
@@ -3477,7 +3475,7 @@
     </row>
     <row r="77" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="2" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B77" s="1" t="s">
         <v>3</v>
@@ -3488,7 +3486,7 @@
     </row>
     <row r="78" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="2" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B78" s="1" t="s">
         <v>4</v>
@@ -3499,7 +3497,7 @@
     </row>
     <row r="79" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="2" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B79" s="1" t="s">
         <v>5</v>
@@ -3510,7 +3508,7 @@
     </row>
     <row r="80" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="2" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B80" s="1" t="s">
         <v>6</v>
@@ -3521,7 +3519,7 @@
     </row>
     <row r="81" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="2" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B81" s="1" t="s">
         <v>7</v>
@@ -3532,7 +3530,7 @@
     </row>
     <row r="82" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="2" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B82" s="1" t="s">
         <v>8</v>
@@ -3543,7 +3541,7 @@
     </row>
     <row r="83" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="2" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B83" s="1" t="s">
         <v>9</v>
@@ -3554,7 +3552,7 @@
     </row>
     <row r="84" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="2" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B84" s="1" t="s">
         <v>10</v>
@@ -3565,7 +3563,7 @@
     </row>
     <row r="85" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="2" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B85" s="1" t="s">
         <v>11</v>
@@ -3576,7 +3574,7 @@
     </row>
     <row r="86" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="2" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B86" s="1" t="s">
         <v>12</v>
@@ -3587,7 +3585,7 @@
     </row>
     <row r="87" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="2" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B87" s="1" t="s">
         <v>13</v>
@@ -3598,7 +3596,7 @@
     </row>
     <row r="88" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="2" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B88" s="1" t="s">
         <v>14</v>
@@ -3609,7 +3607,7 @@
     </row>
     <row r="89" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="2" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B89" s="1" t="s">
         <v>15</v>
@@ -3620,7 +3618,7 @@
     </row>
     <row r="90" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="2" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B90" s="1" t="s">
         <v>16</v>
@@ -3631,7 +3629,7 @@
     </row>
     <row r="91" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="2" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B91" s="1" t="s">
         <v>17</v>
@@ -3642,7 +3640,7 @@
     </row>
     <row r="92" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="2" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B92" s="1" t="s">
         <v>18</v>
@@ -3653,7 +3651,7 @@
     </row>
     <row r="93" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="2" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B93" s="1" t="s">
         <v>19</v>
@@ -3664,7 +3662,7 @@
     </row>
     <row r="94" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="2" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B94" s="1" t="s">
         <v>20</v>
@@ -3675,7 +3673,7 @@
     </row>
     <row r="95" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="2" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B95" s="1" t="s">
         <v>21</v>
@@ -3686,7 +3684,7 @@
     </row>
     <row r="96" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="2" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B96" s="1" t="s">
         <v>22</v>
@@ -3697,7 +3695,7 @@
     </row>
     <row r="97" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="2" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B97" s="1" t="s">
         <v>23</v>

</xml_diff>